<commit_message>
H2 finished except for few minor discrepancies which are still unclear.
</commit_message>
<xml_diff>
--- a/Clarifications/H1 - mandatory data elements.xlsx
+++ b/Clarifications/H1 - mandatory data elements.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28269B9D-EA62-424B-992E-B5F95E5CCFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="14310" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="0" windowWidth="17895" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2402,8 +2402,8 @@
   <dimension ref="A1:I236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6358,8 +6358,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>